<commit_message>
Analysis of fraction correct
</commit_message>
<xml_diff>
--- a/ja512751q_si_003.xlsx
+++ b/ja512751q_si_003.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="0" windowWidth="28680" windowHeight="18220" tabRatio="500" activeTab="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="231">
   <si>
     <t>System</t>
   </si>
@@ -941,24 +941,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1175,7 +1159,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1185,14 +1169,6 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1202,14 +1178,6 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1977,8 +1945,8 @@
   <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A185" sqref="A185:A207"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2047,9 +2015,7 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1">
-      <c r="A3" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="23"/>
       <c r="B3" s="24" t="s">
         <v>23</v>
       </c>
@@ -2075,9 +2041,7 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1">
-      <c r="A4" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="23"/>
       <c r="B4" s="24" t="s">
         <v>24</v>
       </c>
@@ -2103,9 +2067,7 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1">
-      <c r="A5" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="23"/>
       <c r="B5" s="24" t="s">
         <v>25</v>
       </c>
@@ -2131,9 +2093,7 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1">
-      <c r="A6" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="23"/>
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2159,9 +2119,7 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1">
-      <c r="A7" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="23"/>
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2187,9 +2145,7 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1">
-      <c r="A8" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="23"/>
       <c r="B8" s="24" t="s">
         <v>28</v>
       </c>
@@ -2215,9 +2171,7 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1">
-      <c r="A9" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>29</v>
       </c>
@@ -2243,9 +2197,7 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1">
-      <c r="A10" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="23"/>
       <c r="B10" s="24" t="s">
         <v>30</v>
       </c>
@@ -2271,9 +2223,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1">
-      <c r="A11" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="23"/>
       <c r="B11" s="24" t="s">
         <v>31</v>
       </c>
@@ -2299,9 +2249,7 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1">
-      <c r="A12" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
@@ -2327,9 +2275,7 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1">
-      <c r="A13" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A13" s="23"/>
       <c r="B13" s="24" t="s">
         <v>33</v>
       </c>
@@ -2355,9 +2301,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1">
-      <c r="A14" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="23"/>
       <c r="B14" s="24" t="s">
         <v>34</v>
       </c>
@@ -2383,9 +2327,7 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1">
-      <c r="A15" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A15" s="23"/>
       <c r="B15" s="24" t="s">
         <v>35</v>
       </c>
@@ -2411,9 +2353,7 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1">
-      <c r="A16" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A16" s="23"/>
       <c r="B16" s="24" t="s">
         <v>36</v>
       </c>
@@ -2439,9 +2379,7 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1">
-      <c r="A17" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A17" s="23"/>
       <c r="B17" s="24" t="s">
         <v>37</v>
       </c>
@@ -2467,9 +2405,7 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1">
-      <c r="A18" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
         <v>38</v>
       </c>
@@ -2495,9 +2431,7 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
         <v>39</v>
       </c>
@@ -2523,9 +2457,7 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1">
-      <c r="A20" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A20" s="23"/>
       <c r="B20" s="24" t="s">
         <v>40</v>
       </c>
@@ -2551,9 +2483,7 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1">
-      <c r="A21" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A21" s="23"/>
       <c r="B21" s="24" t="s">
         <v>41</v>
       </c>
@@ -2579,9 +2509,7 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1">
-      <c r="A22" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A22" s="23"/>
       <c r="B22" s="24" t="s">
         <v>42</v>
       </c>
@@ -2607,9 +2535,7 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1">
-      <c r="A23" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A23" s="23"/>
       <c r="B23" s="24" t="s">
         <v>43</v>
       </c>
@@ -2635,9 +2561,7 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1">
-      <c r="A24" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A24" s="23"/>
       <c r="B24" s="24" t="s">
         <v>44</v>
       </c>
@@ -2663,9 +2587,7 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1">
-      <c r="A25" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A25" s="23"/>
       <c r="B25" s="24" t="s">
         <v>45</v>
       </c>
@@ -2691,9 +2613,7 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1">
-      <c r="A26" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A26" s="23"/>
       <c r="B26" s="24" t="s">
         <v>46</v>
       </c>
@@ -2719,9 +2639,7 @@
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1">
-      <c r="A27" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A27" s="23"/>
       <c r="B27" s="24" t="s">
         <v>47</v>
       </c>
@@ -2747,9 +2665,7 @@
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1">
-      <c r="A28" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A28" s="23"/>
       <c r="B28" s="24" t="s">
         <v>48</v>
       </c>
@@ -2775,9 +2691,7 @@
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1">
-      <c r="A29" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A29" s="23"/>
       <c r="B29" s="24" t="s">
         <v>49</v>
       </c>
@@ -2803,9 +2717,7 @@
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" s="4" customFormat="1">
-      <c r="A30" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A30" s="23"/>
       <c r="B30" s="24" t="s">
         <v>50</v>
       </c>
@@ -2831,9 +2743,7 @@
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1">
-      <c r="A31" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A31" s="23"/>
       <c r="B31" s="24" t="s">
         <v>51</v>
       </c>
@@ -2859,9 +2769,7 @@
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1">
-      <c r="A32" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A32" s="23"/>
       <c r="B32" s="24" t="s">
         <v>52</v>
       </c>
@@ -2887,9 +2795,7 @@
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1">
-      <c r="A33" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A33" s="23"/>
       <c r="B33" s="24" t="s">
         <v>53</v>
       </c>
@@ -2915,9 +2821,7 @@
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1">
-      <c r="A34" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A34" s="23"/>
       <c r="B34" s="24" t="s">
         <v>54</v>
       </c>
@@ -2943,9 +2847,7 @@
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1">
-      <c r="A35" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A35" s="23"/>
       <c r="B35" s="24" t="s">
         <v>55</v>
       </c>
@@ -2971,9 +2873,7 @@
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1">
-      <c r="A36" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A36" s="23"/>
       <c r="B36" s="24" t="s">
         <v>56</v>
       </c>
@@ -2999,9 +2899,7 @@
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1">
-      <c r="A37" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A37" s="23"/>
       <c r="B37" s="24" t="s">
         <v>57</v>
       </c>
@@ -3066,9 +2964,7 @@
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" s="8" customFormat="1">
-      <c r="A40" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A40" s="25"/>
       <c r="B40" s="26">
         <v>20</v>
       </c>
@@ -3094,9 +2990,7 @@
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" s="8" customFormat="1">
-      <c r="A41" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A41" s="25"/>
       <c r="B41" s="26">
         <v>21</v>
       </c>
@@ -3122,9 +3016,7 @@
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" s="8" customFormat="1">
-      <c r="A42" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A42" s="25"/>
       <c r="B42" s="26">
         <v>22</v>
       </c>
@@ -3150,9 +3042,7 @@
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" s="8" customFormat="1">
-      <c r="A43" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A43" s="25"/>
       <c r="B43" s="26">
         <v>26</v>
       </c>
@@ -3178,9 +3068,7 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" s="8" customFormat="1">
-      <c r="A44" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A44" s="25"/>
       <c r="B44" s="26">
         <v>28</v>
       </c>
@@ -3206,9 +3094,7 @@
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" s="8" customFormat="1">
-      <c r="A45" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A45" s="25"/>
       <c r="B45" s="26">
         <v>29</v>
       </c>
@@ -3234,9 +3120,7 @@
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" s="8" customFormat="1">
-      <c r="A46" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A46" s="25"/>
       <c r="B46" s="26">
         <v>30</v>
       </c>
@@ -3262,9 +3146,7 @@
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" s="8" customFormat="1">
-      <c r="A47" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A47" s="25"/>
       <c r="B47" s="26">
         <v>31</v>
       </c>
@@ -3290,9 +3172,7 @@
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10" s="8" customFormat="1">
-      <c r="A48" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A48" s="25"/>
       <c r="B48" s="26">
         <v>32</v>
       </c>
@@ -3318,9 +3198,7 @@
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" s="8" customFormat="1">
-      <c r="A49" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A49" s="25"/>
       <c r="B49" s="26" t="s">
         <v>58</v>
       </c>
@@ -3346,9 +3224,7 @@
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" s="8" customFormat="1">
-      <c r="A50" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A50" s="25"/>
       <c r="B50" s="26" t="s">
         <v>59</v>
       </c>
@@ -3374,9 +3250,7 @@
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:10" s="8" customFormat="1">
-      <c r="A51" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A51" s="25"/>
       <c r="B51" s="26" t="s">
         <v>60</v>
       </c>
@@ -3402,9 +3276,7 @@
       <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10" s="8" customFormat="1">
-      <c r="A52" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A52" s="25"/>
       <c r="B52" s="26" t="s">
         <v>61</v>
       </c>
@@ -3430,9 +3302,7 @@
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" s="8" customFormat="1">
-      <c r="A53" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A53" s="25"/>
       <c r="B53" s="26" t="s">
         <v>62</v>
       </c>
@@ -3458,9 +3328,7 @@
       <c r="J53" s="7"/>
     </row>
     <row r="54" spans="1:10" s="8" customFormat="1">
-      <c r="A54" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A54" s="25"/>
       <c r="B54" s="26" t="s">
         <v>63</v>
       </c>
@@ -3525,9 +3393,7 @@
       <c r="J56" s="9"/>
     </row>
     <row r="57" spans="1:10" s="10" customFormat="1">
-      <c r="A57" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A57" s="27"/>
       <c r="B57" s="28" t="s">
         <v>65</v>
       </c>
@@ -3553,9 +3419,7 @@
       <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:10" s="10" customFormat="1">
-      <c r="A58" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A58" s="27"/>
       <c r="B58" s="28" t="s">
         <v>66</v>
       </c>
@@ -3581,9 +3445,7 @@
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="1:10" s="10" customFormat="1">
-      <c r="A59" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A59" s="27"/>
       <c r="B59" s="28" t="s">
         <v>67</v>
       </c>
@@ -3609,9 +3471,7 @@
       <c r="J59" s="9"/>
     </row>
     <row r="60" spans="1:10" s="10" customFormat="1">
-      <c r="A60" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A60" s="27"/>
       <c r="B60" s="28" t="s">
         <v>68</v>
       </c>
@@ -3637,9 +3497,7 @@
       <c r="J60" s="9"/>
     </row>
     <row r="61" spans="1:10" s="10" customFormat="1">
-      <c r="A61" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A61" s="27"/>
       <c r="B61" s="28" t="s">
         <v>69</v>
       </c>
@@ -3665,9 +3523,7 @@
       <c r="J61" s="9"/>
     </row>
     <row r="62" spans="1:10" s="10" customFormat="1">
-      <c r="A62" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A62" s="27"/>
       <c r="B62" s="28" t="s">
         <v>70</v>
       </c>
@@ -3693,9 +3549,7 @@
       <c r="J62" s="9"/>
     </row>
     <row r="63" spans="1:10" s="10" customFormat="1">
-      <c r="A63" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A63" s="27"/>
       <c r="B63" s="28" t="s">
         <v>71</v>
       </c>
@@ -3721,9 +3575,7 @@
       <c r="J63" s="9"/>
     </row>
     <row r="64" spans="1:10" s="10" customFormat="1">
-      <c r="A64" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A64" s="27"/>
       <c r="B64" s="28" t="s">
         <v>72</v>
       </c>
@@ -3749,9 +3601,7 @@
       <c r="J64" s="9"/>
     </row>
     <row r="65" spans="1:10" s="10" customFormat="1">
-      <c r="A65" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A65" s="27"/>
       <c r="B65" s="28" t="s">
         <v>73</v>
       </c>
@@ -3777,9 +3627,7 @@
       <c r="J65" s="9"/>
     </row>
     <row r="66" spans="1:10" s="10" customFormat="1">
-      <c r="A66" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A66" s="27"/>
       <c r="B66" s="28" t="s">
         <v>74</v>
       </c>
@@ -3805,9 +3653,7 @@
       <c r="J66" s="9"/>
     </row>
     <row r="67" spans="1:10" s="10" customFormat="1">
-      <c r="A67" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A67" s="27"/>
       <c r="B67" s="28" t="s">
         <v>75</v>
       </c>
@@ -3833,9 +3679,7 @@
       <c r="J67" s="9"/>
     </row>
     <row r="68" spans="1:10" s="10" customFormat="1">
-      <c r="A68" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A68" s="27"/>
       <c r="B68" s="28" t="s">
         <v>76</v>
       </c>
@@ -3861,9 +3705,7 @@
       <c r="J68" s="9"/>
     </row>
     <row r="69" spans="1:10" s="10" customFormat="1">
-      <c r="A69" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A69" s="27"/>
       <c r="B69" s="28" t="s">
         <v>77</v>
       </c>
@@ -3889,9 +3731,7 @@
       <c r="J69" s="9"/>
     </row>
     <row r="70" spans="1:10" s="10" customFormat="1">
-      <c r="A70" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A70" s="27"/>
       <c r="B70" s="28" t="s">
         <v>78</v>
       </c>
@@ -3917,9 +3757,7 @@
       <c r="J70" s="9"/>
     </row>
     <row r="71" spans="1:10" s="10" customFormat="1">
-      <c r="A71" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A71" s="27"/>
       <c r="B71" s="28" t="s">
         <v>79</v>
       </c>
@@ -3945,9 +3783,7 @@
       <c r="J71" s="9"/>
     </row>
     <row r="72" spans="1:10" s="10" customFormat="1">
-      <c r="A72" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A72" s="27"/>
       <c r="B72" s="28" t="s">
         <v>80</v>
       </c>
@@ -3973,9 +3809,7 @@
       <c r="J72" s="9"/>
     </row>
     <row r="73" spans="1:10" s="10" customFormat="1">
-      <c r="A73" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A73" s="27"/>
       <c r="B73" s="28" t="s">
         <v>81</v>
       </c>
@@ -4001,9 +3835,7 @@
       <c r="J73" s="9"/>
     </row>
     <row r="74" spans="1:10" s="10" customFormat="1">
-      <c r="A74" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A74" s="27"/>
       <c r="B74" s="28" t="s">
         <v>82</v>
       </c>
@@ -4029,9 +3861,7 @@
       <c r="J74" s="9"/>
     </row>
     <row r="75" spans="1:10" s="10" customFormat="1">
-      <c r="A75" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A75" s="27"/>
       <c r="B75" s="28" t="s">
         <v>83</v>
       </c>
@@ -4057,9 +3887,7 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" spans="1:10" s="10" customFormat="1">
-      <c r="A76" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="A76" s="27"/>
       <c r="B76" s="28" t="s">
         <v>84</v>
       </c>
@@ -4124,9 +3952,7 @@
       <c r="J78" s="20"/>
     </row>
     <row r="79" spans="1:10" s="19" customFormat="1">
-      <c r="A79" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A79" s="29"/>
       <c r="B79" s="30">
         <v>26</v>
       </c>
@@ -4152,9 +3978,7 @@
       <c r="J79" s="20"/>
     </row>
     <row r="80" spans="1:10" s="19" customFormat="1">
-      <c r="A80" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A80" s="29"/>
       <c r="B80" s="30">
         <v>27</v>
       </c>
@@ -4180,9 +4004,7 @@
       <c r="J80" s="20"/>
     </row>
     <row r="81" spans="1:10" s="19" customFormat="1">
-      <c r="A81" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A81" s="29"/>
       <c r="B81" s="30">
         <v>28</v>
       </c>
@@ -4208,9 +4030,7 @@
       <c r="J81" s="20"/>
     </row>
     <row r="82" spans="1:10" s="19" customFormat="1">
-      <c r="A82" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A82" s="29"/>
       <c r="B82" s="30">
         <v>29</v>
       </c>
@@ -4236,9 +4056,7 @@
       <c r="J82" s="20"/>
     </row>
     <row r="83" spans="1:10" s="19" customFormat="1">
-      <c r="A83" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A83" s="29"/>
       <c r="B83" s="30">
         <v>30</v>
       </c>
@@ -4264,9 +4082,7 @@
       <c r="J83" s="20"/>
     </row>
     <row r="84" spans="1:10" s="19" customFormat="1">
-      <c r="A84" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A84" s="29"/>
       <c r="B84" s="30">
         <v>31</v>
       </c>
@@ -4292,9 +4108,7 @@
       <c r="J84" s="20"/>
     </row>
     <row r="85" spans="1:10" s="19" customFormat="1">
-      <c r="A85" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A85" s="29"/>
       <c r="B85" s="30">
         <v>32</v>
       </c>
@@ -4320,9 +4134,7 @@
       <c r="J85" s="20"/>
     </row>
     <row r="86" spans="1:10" s="19" customFormat="1">
-      <c r="A86" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A86" s="29"/>
       <c r="B86" s="30">
         <v>33</v>
       </c>
@@ -4348,9 +4160,7 @@
       <c r="J86" s="20"/>
     </row>
     <row r="87" spans="1:10" s="19" customFormat="1">
-      <c r="A87" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A87" s="29"/>
       <c r="B87" s="30">
         <v>34</v>
       </c>
@@ -4376,9 +4186,7 @@
       <c r="J87" s="20"/>
     </row>
     <row r="88" spans="1:10" s="19" customFormat="1">
-      <c r="A88" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A88" s="29"/>
       <c r="B88" s="30">
         <v>35</v>
       </c>
@@ -4404,9 +4212,7 @@
       <c r="J88" s="20"/>
     </row>
     <row r="89" spans="1:10" s="19" customFormat="1">
-      <c r="A89" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A89" s="29"/>
       <c r="B89" s="30">
         <v>36</v>
       </c>
@@ -4432,9 +4238,7 @@
       <c r="J89" s="20"/>
     </row>
     <row r="90" spans="1:10" s="19" customFormat="1">
-      <c r="A90" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A90" s="29"/>
       <c r="B90" s="30">
         <v>37</v>
       </c>
@@ -4460,9 +4264,7 @@
       <c r="J90" s="20"/>
     </row>
     <row r="91" spans="1:10" s="19" customFormat="1">
-      <c r="A91" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A91" s="29"/>
       <c r="B91" s="30">
         <v>38</v>
       </c>
@@ -4488,9 +4290,7 @@
       <c r="J91" s="20"/>
     </row>
     <row r="92" spans="1:10" s="19" customFormat="1">
-      <c r="A92" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A92" s="29"/>
       <c r="B92" s="30">
         <v>39</v>
       </c>
@@ -4516,9 +4316,7 @@
       <c r="J92" s="20"/>
     </row>
     <row r="93" spans="1:10" s="19" customFormat="1">
-      <c r="A93" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A93" s="29"/>
       <c r="B93" s="30">
         <v>40</v>
       </c>
@@ -4544,9 +4342,7 @@
       <c r="J93" s="20"/>
     </row>
     <row r="94" spans="1:10" s="19" customFormat="1">
-      <c r="A94" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A94" s="29"/>
       <c r="B94" s="30">
         <v>41</v>
       </c>
@@ -4572,9 +4368,7 @@
       <c r="J94" s="20"/>
     </row>
     <row r="95" spans="1:10" s="19" customFormat="1">
-      <c r="A95" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A95" s="29"/>
       <c r="B95" s="30">
         <v>42</v>
       </c>
@@ -4600,9 +4394,7 @@
       <c r="J95" s="20"/>
     </row>
     <row r="96" spans="1:10" s="19" customFormat="1">
-      <c r="A96" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A96" s="29"/>
       <c r="B96" s="30">
         <v>43</v>
       </c>
@@ -4628,9 +4420,7 @@
       <c r="J96" s="20"/>
     </row>
     <row r="97" spans="1:10" s="19" customFormat="1">
-      <c r="A97" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A97" s="29"/>
       <c r="B97" s="30">
         <v>44</v>
       </c>
@@ -4656,9 +4446,7 @@
       <c r="J97" s="20"/>
     </row>
     <row r="98" spans="1:10" s="19" customFormat="1">
-      <c r="A98" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A98" s="29"/>
       <c r="B98" s="30">
         <v>45</v>
       </c>
@@ -4684,9 +4472,7 @@
       <c r="J98" s="20"/>
     </row>
     <row r="99" spans="1:10" s="19" customFormat="1">
-      <c r="A99" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A99" s="29"/>
       <c r="B99" s="30">
         <v>46</v>
       </c>
@@ -4712,9 +4498,7 @@
       <c r="J99" s="20"/>
     </row>
     <row r="100" spans="1:10" s="19" customFormat="1">
-      <c r="A100" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A100" s="29"/>
       <c r="B100" s="30">
         <v>47</v>
       </c>
@@ -4740,9 +4524,7 @@
       <c r="J100" s="20"/>
     </row>
     <row r="101" spans="1:10" s="19" customFormat="1">
-      <c r="A101" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A101" s="29"/>
       <c r="B101" s="30">
         <v>48</v>
       </c>
@@ -4768,9 +4550,7 @@
       <c r="J101" s="20"/>
     </row>
     <row r="102" spans="1:10" s="19" customFormat="1">
-      <c r="A102" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A102" s="29"/>
       <c r="B102" s="30">
         <v>49</v>
       </c>
@@ -4796,9 +4576,7 @@
       <c r="J102" s="20"/>
     </row>
     <row r="103" spans="1:10" s="19" customFormat="1">
-      <c r="A103" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A103" s="29"/>
       <c r="B103" s="30">
         <v>50</v>
       </c>
@@ -4824,9 +4602,7 @@
       <c r="J103" s="20"/>
     </row>
     <row r="104" spans="1:10" s="19" customFormat="1">
-      <c r="A104" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A104" s="29"/>
       <c r="B104" s="30">
         <v>51</v>
       </c>
@@ -4852,9 +4628,7 @@
       <c r="J104" s="20"/>
     </row>
     <row r="105" spans="1:10" s="19" customFormat="1">
-      <c r="A105" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A105" s="29"/>
       <c r="B105" s="30">
         <v>52</v>
       </c>
@@ -4880,9 +4654,7 @@
       <c r="J105" s="20"/>
     </row>
     <row r="106" spans="1:10" s="19" customFormat="1">
-      <c r="A106" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A106" s="29"/>
       <c r="B106" s="30">
         <v>53</v>
       </c>
@@ -4908,9 +4680,7 @@
       <c r="J106" s="20"/>
     </row>
     <row r="107" spans="1:10" s="19" customFormat="1">
-      <c r="A107" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A107" s="29"/>
       <c r="B107" s="30">
         <v>54</v>
       </c>
@@ -4936,9 +4706,7 @@
       <c r="J107" s="20"/>
     </row>
     <row r="108" spans="1:10" s="19" customFormat="1">
-      <c r="A108" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A108" s="29"/>
       <c r="B108" s="30">
         <v>56</v>
       </c>
@@ -4964,9 +4732,7 @@
       <c r="J108" s="20"/>
     </row>
     <row r="109" spans="1:10" s="19" customFormat="1">
-      <c r="A109" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A109" s="29"/>
       <c r="B109" s="30">
         <v>57</v>
       </c>
@@ -4992,9 +4758,7 @@
       <c r="J109" s="20"/>
     </row>
     <row r="110" spans="1:10" s="19" customFormat="1">
-      <c r="A110" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A110" s="29"/>
       <c r="B110" s="30">
         <v>58</v>
       </c>
@@ -5020,9 +4784,7 @@
       <c r="J110" s="20"/>
     </row>
     <row r="111" spans="1:10" s="19" customFormat="1">
-      <c r="A111" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A111" s="29"/>
       <c r="B111" s="30">
         <v>60</v>
       </c>
@@ -5048,9 +4810,7 @@
       <c r="J111" s="20"/>
     </row>
     <row r="112" spans="1:10" s="19" customFormat="1">
-      <c r="A112" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A112" s="29"/>
       <c r="B112" s="30">
         <v>61</v>
       </c>
@@ -5076,9 +4836,7 @@
       <c r="J112" s="20"/>
     </row>
     <row r="113" spans="1:10" s="19" customFormat="1">
-      <c r="A113" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A113" s="29"/>
       <c r="B113" s="30">
         <v>62</v>
       </c>
@@ -5104,9 +4862,7 @@
       <c r="J113" s="20"/>
     </row>
     <row r="114" spans="1:10" s="19" customFormat="1">
-      <c r="A114" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A114" s="29"/>
       <c r="B114" s="30">
         <v>63</v>
       </c>
@@ -5132,9 +4888,7 @@
       <c r="J114" s="20"/>
     </row>
     <row r="115" spans="1:10" s="19" customFormat="1">
-      <c r="A115" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A115" s="29"/>
       <c r="B115" s="30">
         <v>64</v>
       </c>
@@ -5160,9 +4914,7 @@
       <c r="J115" s="20"/>
     </row>
     <row r="116" spans="1:10" s="19" customFormat="1">
-      <c r="A116" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A116" s="29"/>
       <c r="B116" s="30">
         <v>65</v>
       </c>
@@ -5188,9 +4940,7 @@
       <c r="J116" s="20"/>
     </row>
     <row r="117" spans="1:10" s="19" customFormat="1">
-      <c r="A117" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A117" s="29"/>
       <c r="B117" s="30">
         <v>66</v>
       </c>
@@ -5216,9 +4966,7 @@
       <c r="J117" s="20"/>
     </row>
     <row r="118" spans="1:10" s="19" customFormat="1">
-      <c r="A118" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A118" s="29"/>
       <c r="B118" s="30">
         <v>67</v>
       </c>
@@ -5244,9 +4992,7 @@
       <c r="J118" s="20"/>
     </row>
     <row r="119" spans="1:10" s="19" customFormat="1">
-      <c r="A119" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A119" s="29"/>
       <c r="B119" s="30">
         <v>68</v>
       </c>
@@ -5311,9 +5057,7 @@
       <c r="J121" s="14"/>
     </row>
     <row r="122" spans="1:10" s="15" customFormat="1">
-      <c r="A122" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A122" s="31"/>
       <c r="B122" s="32" t="s">
         <v>86</v>
       </c>
@@ -5339,9 +5083,7 @@
       <c r="J122" s="14"/>
     </row>
     <row r="123" spans="1:10" s="15" customFormat="1">
-      <c r="A123" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A123" s="31"/>
       <c r="B123" s="32" t="s">
         <v>87</v>
       </c>
@@ -5367,9 +5109,7 @@
       <c r="J123" s="14"/>
     </row>
     <row r="124" spans="1:10" s="15" customFormat="1">
-      <c r="A124" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A124" s="31"/>
       <c r="B124" s="32" t="s">
         <v>88</v>
       </c>
@@ -5395,9 +5135,7 @@
       <c r="J124" s="14"/>
     </row>
     <row r="125" spans="1:10" s="15" customFormat="1">
-      <c r="A125" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A125" s="31"/>
       <c r="B125" s="32" t="s">
         <v>89</v>
       </c>
@@ -5423,9 +5161,7 @@
       <c r="J125" s="14"/>
     </row>
     <row r="126" spans="1:10" s="15" customFormat="1">
-      <c r="A126" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A126" s="31"/>
       <c r="B126" s="32" t="s">
         <v>90</v>
       </c>
@@ -5451,9 +5187,7 @@
       <c r="J126" s="14"/>
     </row>
     <row r="127" spans="1:10" s="15" customFormat="1">
-      <c r="A127" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A127" s="31"/>
       <c r="B127" s="32" t="s">
         <v>91</v>
       </c>
@@ -5479,9 +5213,7 @@
       <c r="J127" s="14"/>
     </row>
     <row r="128" spans="1:10" s="15" customFormat="1">
-      <c r="A128" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A128" s="31"/>
       <c r="B128" s="32" t="s">
         <v>92</v>
       </c>
@@ -5507,9 +5239,7 @@
       <c r="J128" s="14"/>
     </row>
     <row r="129" spans="1:10" s="15" customFormat="1">
-      <c r="A129" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A129" s="31"/>
       <c r="B129" s="32" t="s">
         <v>93</v>
       </c>
@@ -5535,9 +5265,7 @@
       <c r="J129" s="14"/>
     </row>
     <row r="130" spans="1:10" s="15" customFormat="1">
-      <c r="A130" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A130" s="31"/>
       <c r="B130" s="32" t="s">
         <v>94</v>
       </c>
@@ -5563,9 +5291,7 @@
       <c r="J130" s="14"/>
     </row>
     <row r="131" spans="1:10" s="15" customFormat="1">
-      <c r="A131" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A131" s="31"/>
       <c r="B131" s="32" t="s">
         <v>95</v>
       </c>
@@ -5591,9 +5317,7 @@
       <c r="J131" s="14"/>
     </row>
     <row r="132" spans="1:10" s="15" customFormat="1">
-      <c r="A132" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A132" s="31"/>
       <c r="B132" s="32" t="s">
         <v>96</v>
       </c>
@@ -5619,9 +5343,7 @@
       <c r="J132" s="14"/>
     </row>
     <row r="133" spans="1:10" s="15" customFormat="1">
-      <c r="A133" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A133" s="31"/>
       <c r="B133" s="32" t="s">
         <v>97</v>
       </c>
@@ -5647,9 +5369,7 @@
       <c r="J133" s="14"/>
     </row>
     <row r="134" spans="1:10" s="15" customFormat="1">
-      <c r="A134" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A134" s="31"/>
       <c r="B134" s="32" t="s">
         <v>98</v>
       </c>
@@ -5675,9 +5395,7 @@
       <c r="J134" s="14"/>
     </row>
     <row r="135" spans="1:10" s="15" customFormat="1">
-      <c r="A135" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A135" s="31"/>
       <c r="B135" s="32" t="s">
         <v>99</v>
       </c>
@@ -5703,9 +5421,7 @@
       <c r="J135" s="14"/>
     </row>
     <row r="136" spans="1:10" s="15" customFormat="1">
-      <c r="A136" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A136" s="31"/>
       <c r="B136" s="32" t="s">
         <v>100</v>
       </c>
@@ -5731,9 +5447,7 @@
       <c r="J136" s="14"/>
     </row>
     <row r="137" spans="1:10" s="15" customFormat="1">
-      <c r="A137" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A137" s="31"/>
       <c r="B137" s="32" t="s">
         <v>101</v>
       </c>
@@ -5759,9 +5473,7 @@
       <c r="J137" s="14"/>
     </row>
     <row r="138" spans="1:10" s="15" customFormat="1">
-      <c r="A138" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A138" s="31"/>
       <c r="B138" s="32" t="s">
         <v>102</v>
       </c>
@@ -5787,9 +5499,7 @@
       <c r="J138" s="14"/>
     </row>
     <row r="139" spans="1:10" s="15" customFormat="1">
-      <c r="A139" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A139" s="31"/>
       <c r="B139" s="32" t="s">
         <v>103</v>
       </c>
@@ -5815,9 +5525,7 @@
       <c r="J139" s="14"/>
     </row>
     <row r="140" spans="1:10" s="15" customFormat="1">
-      <c r="A140" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A140" s="31"/>
       <c r="B140" s="32" t="s">
         <v>104</v>
       </c>
@@ -5843,9 +5551,7 @@
       <c r="J140" s="14"/>
     </row>
     <row r="141" spans="1:10" s="15" customFormat="1">
-      <c r="A141" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A141" s="31"/>
       <c r="B141" s="32" t="s">
         <v>105</v>
       </c>
@@ -5871,9 +5577,7 @@
       <c r="J141" s="14"/>
     </row>
     <row r="142" spans="1:10" s="15" customFormat="1">
-      <c r="A142" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A142" s="31"/>
       <c r="B142" s="32" t="s">
         <v>106</v>
       </c>
@@ -5899,9 +5603,7 @@
       <c r="J142" s="14"/>
     </row>
     <row r="143" spans="1:10" s="15" customFormat="1">
-      <c r="A143" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A143" s="31"/>
       <c r="B143" s="32" t="s">
         <v>107</v>
       </c>
@@ -5927,9 +5629,7 @@
       <c r="J143" s="14"/>
     </row>
     <row r="144" spans="1:10" s="15" customFormat="1">
-      <c r="A144" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A144" s="31"/>
       <c r="B144" s="32" t="s">
         <v>108</v>
       </c>
@@ -5955,9 +5655,7 @@
       <c r="J144" s="14"/>
     </row>
     <row r="145" spans="1:10" s="15" customFormat="1">
-      <c r="A145" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A145" s="31"/>
       <c r="B145" s="32" t="s">
         <v>109</v>
       </c>
@@ -5983,9 +5681,7 @@
       <c r="J145" s="14"/>
     </row>
     <row r="146" spans="1:10" s="15" customFormat="1">
-      <c r="A146" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A146" s="31"/>
       <c r="B146" s="32" t="s">
         <v>110</v>
       </c>
@@ -6011,9 +5707,7 @@
       <c r="J146" s="14"/>
     </row>
     <row r="147" spans="1:10" s="15" customFormat="1">
-      <c r="A147" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A147" s="31"/>
       <c r="B147" s="32" t="s">
         <v>111</v>
       </c>
@@ -6039,9 +5733,7 @@
       <c r="J147" s="14"/>
     </row>
     <row r="148" spans="1:10" s="15" customFormat="1">
-      <c r="A148" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A148" s="31"/>
       <c r="B148" s="32" t="s">
         <v>112</v>
       </c>
@@ -6067,9 +5759,7 @@
       <c r="J148" s="14"/>
     </row>
     <row r="149" spans="1:10" s="15" customFormat="1">
-      <c r="A149" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A149" s="31"/>
       <c r="B149" s="32" t="s">
         <v>113</v>
       </c>
@@ -6095,9 +5785,7 @@
       <c r="J149" s="14"/>
     </row>
     <row r="150" spans="1:10" s="15" customFormat="1">
-      <c r="A150" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A150" s="31"/>
       <c r="B150" s="32" t="s">
         <v>114</v>
       </c>
@@ -6123,9 +5811,7 @@
       <c r="J150" s="14"/>
     </row>
     <row r="151" spans="1:10" s="15" customFormat="1">
-      <c r="A151" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A151" s="31"/>
       <c r="B151" s="32" t="s">
         <v>115</v>
       </c>
@@ -6151,9 +5837,7 @@
       <c r="J151" s="14"/>
     </row>
     <row r="152" spans="1:10" s="15" customFormat="1">
-      <c r="A152" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A152" s="31"/>
       <c r="B152" s="32" t="s">
         <v>116</v>
       </c>
@@ -6179,9 +5863,7 @@
       <c r="J152" s="14"/>
     </row>
     <row r="153" spans="1:10" s="15" customFormat="1">
-      <c r="A153" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A153" s="31"/>
       <c r="B153" s="32" t="s">
         <v>117</v>
       </c>
@@ -6207,9 +5889,7 @@
       <c r="J153" s="14"/>
     </row>
     <row r="154" spans="1:10" s="15" customFormat="1">
-      <c r="A154" s="31" t="s">
-        <v>182</v>
-      </c>
+      <c r="A154" s="31"/>
       <c r="B154" s="32" t="s">
         <v>118</v>
       </c>
@@ -6274,9 +5954,7 @@
       <c r="J156" s="9"/>
     </row>
     <row r="157" spans="1:10" s="10" customFormat="1">
-      <c r="A157" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A157" s="27"/>
       <c r="B157" s="28">
         <v>5</v>
       </c>
@@ -6302,9 +5980,7 @@
       <c r="J157" s="9"/>
     </row>
     <row r="158" spans="1:10" s="10" customFormat="1">
-      <c r="A158" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A158" s="27"/>
       <c r="B158" s="28" t="s">
         <v>120</v>
       </c>
@@ -6330,9 +6006,7 @@
       <c r="J158" s="9"/>
     </row>
     <row r="159" spans="1:10" s="10" customFormat="1">
-      <c r="A159" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A159" s="27"/>
       <c r="B159" s="28" t="s">
         <v>121</v>
       </c>
@@ -6358,9 +6032,7 @@
       <c r="J159" s="9"/>
     </row>
     <row r="160" spans="1:10" s="10" customFormat="1">
-      <c r="A160" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A160" s="27"/>
       <c r="B160" s="28" t="s">
         <v>122</v>
       </c>
@@ -6386,9 +6058,7 @@
       <c r="J160" s="9"/>
     </row>
     <row r="161" spans="1:10" s="10" customFormat="1">
-      <c r="A161" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A161" s="27"/>
       <c r="B161" s="28" t="s">
         <v>123</v>
       </c>
@@ -6414,9 +6084,7 @@
       <c r="J161" s="9"/>
     </row>
     <row r="162" spans="1:10" s="10" customFormat="1">
-      <c r="A162" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A162" s="27"/>
       <c r="B162" s="28" t="s">
         <v>124</v>
       </c>
@@ -6442,9 +6110,7 @@
       <c r="J162" s="9"/>
     </row>
     <row r="163" spans="1:10" s="10" customFormat="1">
-      <c r="A163" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A163" s="27"/>
       <c r="B163" s="28" t="s">
         <v>125</v>
       </c>
@@ -6470,9 +6136,7 @@
       <c r="J163" s="9"/>
     </row>
     <row r="164" spans="1:10" s="10" customFormat="1">
-      <c r="A164" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A164" s="27"/>
       <c r="B164" s="28" t="s">
         <v>126</v>
       </c>
@@ -6498,9 +6162,7 @@
       <c r="J164" s="9"/>
     </row>
     <row r="165" spans="1:10" s="10" customFormat="1">
-      <c r="A165" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A165" s="27"/>
       <c r="B165" s="28" t="s">
         <v>127</v>
       </c>
@@ -6526,9 +6188,7 @@
       <c r="J165" s="9"/>
     </row>
     <row r="166" spans="1:10" s="10" customFormat="1">
-      <c r="A166" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A166" s="27"/>
       <c r="B166" s="28" t="s">
         <v>128</v>
       </c>
@@ -6593,9 +6253,7 @@
       <c r="J168" s="16"/>
     </row>
     <row r="169" spans="1:10" s="17" customFormat="1">
-      <c r="A169" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A169" s="33"/>
       <c r="B169" s="34" t="s">
         <v>130</v>
       </c>
@@ -6621,9 +6279,7 @@
       <c r="J169" s="16"/>
     </row>
     <row r="170" spans="1:10" s="17" customFormat="1">
-      <c r="A170" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A170" s="33"/>
       <c r="B170" s="34" t="s">
         <v>131</v>
       </c>
@@ -6649,9 +6305,7 @@
       <c r="J170" s="16"/>
     </row>
     <row r="171" spans="1:10" s="17" customFormat="1">
-      <c r="A171" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A171" s="33"/>
       <c r="B171" s="34" t="s">
         <v>132</v>
       </c>
@@ -6677,9 +6331,7 @@
       <c r="J171" s="16"/>
     </row>
     <row r="172" spans="1:10" s="17" customFormat="1">
-      <c r="A172" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A172" s="33"/>
       <c r="B172" s="34" t="s">
         <v>133</v>
       </c>
@@ -6705,9 +6357,7 @@
       <c r="J172" s="16"/>
     </row>
     <row r="173" spans="1:10" s="17" customFormat="1">
-      <c r="A173" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A173" s="33"/>
       <c r="B173" s="34" t="s">
         <v>134</v>
       </c>
@@ -6733,9 +6383,7 @@
       <c r="J173" s="16"/>
     </row>
     <row r="174" spans="1:10" s="17" customFormat="1">
-      <c r="A174" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A174" s="33"/>
       <c r="B174" s="34" t="s">
         <v>135</v>
       </c>
@@ -6761,9 +6409,7 @@
       <c r="J174" s="16"/>
     </row>
     <row r="175" spans="1:10" s="17" customFormat="1">
-      <c r="A175" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A175" s="33"/>
       <c r="B175" s="34" t="s">
         <v>136</v>
       </c>
@@ -6789,9 +6435,7 @@
       <c r="J175" s="16"/>
     </row>
     <row r="176" spans="1:10" s="17" customFormat="1">
-      <c r="A176" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A176" s="33"/>
       <c r="B176" s="34" t="s">
         <v>137</v>
       </c>
@@ -6817,9 +6461,7 @@
       <c r="J176" s="16"/>
     </row>
     <row r="177" spans="1:10" s="17" customFormat="1">
-      <c r="A177" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A177" s="33"/>
       <c r="B177" s="34" t="s">
         <v>138</v>
       </c>
@@ -6845,9 +6487,7 @@
       <c r="J177" s="16"/>
     </row>
     <row r="178" spans="1:10" s="17" customFormat="1">
-      <c r="A178" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A178" s="33"/>
       <c r="B178" s="34" t="s">
         <v>139</v>
       </c>
@@ -6873,9 +6513,7 @@
       <c r="J178" s="16"/>
     </row>
     <row r="179" spans="1:10" s="17" customFormat="1">
-      <c r="A179" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A179" s="33"/>
       <c r="B179" s="34" t="s">
         <v>140</v>
       </c>
@@ -6901,9 +6539,7 @@
       <c r="J179" s="16"/>
     </row>
     <row r="180" spans="1:10" s="17" customFormat="1">
-      <c r="A180" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A180" s="33"/>
       <c r="B180" s="34" t="s">
         <v>141</v>
       </c>
@@ -6929,9 +6565,7 @@
       <c r="J180" s="16"/>
     </row>
     <row r="181" spans="1:10" s="17" customFormat="1">
-      <c r="A181" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A181" s="33"/>
       <c r="B181" s="34" t="s">
         <v>142</v>
       </c>
@@ -6957,9 +6591,7 @@
       <c r="J181" s="16"/>
     </row>
     <row r="182" spans="1:10" s="17" customFormat="1">
-      <c r="A182" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A182" s="33"/>
       <c r="B182" s="34" t="s">
         <v>143</v>
       </c>
@@ -6985,9 +6617,7 @@
       <c r="J182" s="16"/>
     </row>
     <row r="183" spans="1:10" s="17" customFormat="1">
-      <c r="A183" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="A183" s="33"/>
       <c r="B183" s="34" t="s">
         <v>144</v>
       </c>
@@ -7040,9 +6670,7 @@
       </c>
     </row>
     <row r="186" spans="1:10" s="18" customFormat="1">
-      <c r="A186" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A186" s="35"/>
       <c r="B186" s="36">
         <v>23467</v>
       </c>
@@ -7067,9 +6695,7 @@
       </c>
     </row>
     <row r="187" spans="1:10" s="18" customFormat="1">
-      <c r="A187" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A187" s="35"/>
       <c r="B187" s="36">
         <v>23468</v>
       </c>
@@ -7094,9 +6720,7 @@
       </c>
     </row>
     <row r="188" spans="1:10" s="18" customFormat="1">
-      <c r="A188" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A188" s="35"/>
       <c r="B188" s="36">
         <v>23469</v>
       </c>
@@ -7121,9 +6745,7 @@
       </c>
     </row>
     <row r="189" spans="1:10" s="18" customFormat="1">
-      <c r="A189" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A189" s="35"/>
       <c r="B189" s="36">
         <v>23470</v>
       </c>
@@ -7148,9 +6770,7 @@
       </c>
     </row>
     <row r="190" spans="1:10" s="18" customFormat="1">
-      <c r="A190" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A190" s="35"/>
       <c r="B190" s="36">
         <v>23471</v>
       </c>
@@ -7175,9 +6795,7 @@
       </c>
     </row>
     <row r="191" spans="1:10" s="18" customFormat="1">
-      <c r="A191" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A191" s="35"/>
       <c r="B191" s="36">
         <v>23472</v>
       </c>
@@ -7202,9 +6820,7 @@
       </c>
     </row>
     <row r="192" spans="1:10" s="18" customFormat="1">
-      <c r="A192" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A192" s="35"/>
       <c r="B192" s="36">
         <v>23473</v>
       </c>
@@ -7229,9 +6845,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" s="18" customFormat="1">
-      <c r="A193" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A193" s="35"/>
       <c r="B193" s="36">
         <v>23474</v>
       </c>
@@ -7256,9 +6870,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" s="18" customFormat="1">
-      <c r="A194" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A194" s="35"/>
       <c r="B194" s="36">
         <v>23475</v>
       </c>
@@ -7283,9 +6895,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" s="18" customFormat="1">
-      <c r="A195" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A195" s="35"/>
       <c r="B195" s="36">
         <v>23476</v>
       </c>
@@ -7310,9 +6920,7 @@
       </c>
     </row>
     <row r="196" spans="1:9" s="18" customFormat="1">
-      <c r="A196" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A196" s="35"/>
       <c r="B196" s="36">
         <v>23477</v>
       </c>
@@ -7337,9 +6945,7 @@
       </c>
     </row>
     <row r="197" spans="1:9" s="18" customFormat="1">
-      <c r="A197" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A197" s="35"/>
       <c r="B197" s="36">
         <v>23479</v>
       </c>
@@ -7364,9 +6970,7 @@
       </c>
     </row>
     <row r="198" spans="1:9" s="18" customFormat="1">
-      <c r="A198" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A198" s="35"/>
       <c r="B198" s="36">
         <v>23480</v>
       </c>
@@ -7391,9 +6995,7 @@
       </c>
     </row>
     <row r="199" spans="1:9" s="18" customFormat="1">
-      <c r="A199" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A199" s="35"/>
       <c r="B199" s="36">
         <v>23482</v>
       </c>
@@ -7418,9 +7020,7 @@
       </c>
     </row>
     <row r="200" spans="1:9" s="18" customFormat="1">
-      <c r="A200" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A200" s="35"/>
       <c r="B200" s="36">
         <v>23483</v>
       </c>
@@ -7445,9 +7045,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" s="18" customFormat="1">
-      <c r="A201" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A201" s="35"/>
       <c r="B201" s="36">
         <v>23484</v>
       </c>
@@ -7472,9 +7070,7 @@
       </c>
     </row>
     <row r="202" spans="1:9" s="18" customFormat="1">
-      <c r="A202" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A202" s="35"/>
       <c r="B202" s="36">
         <v>23485</v>
       </c>
@@ -7499,9 +7095,7 @@
       </c>
     </row>
     <row r="203" spans="1:9" s="18" customFormat="1">
-      <c r="A203" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A203" s="35"/>
       <c r="B203" s="36">
         <v>23486</v>
       </c>
@@ -7526,9 +7120,7 @@
       </c>
     </row>
     <row r="204" spans="1:9" s="18" customFormat="1">
-      <c r="A204" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A204" s="35"/>
       <c r="B204" s="36" t="s">
         <v>153</v>
       </c>
@@ -7553,9 +7145,7 @@
       </c>
     </row>
     <row r="205" spans="1:9" s="18" customFormat="1">
-      <c r="A205" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A205" s="35"/>
       <c r="B205" s="36" t="s">
         <v>152</v>
       </c>
@@ -7580,9 +7170,7 @@
       </c>
     </row>
     <row r="206" spans="1:9" s="18" customFormat="1">
-      <c r="A206" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A206" s="35"/>
       <c r="B206" s="36" t="s">
         <v>154</v>
       </c>
@@ -7607,9 +7195,7 @@
       </c>
     </row>
     <row r="207" spans="1:9" s="18" customFormat="1">
-      <c r="A207" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="A207" s="35"/>
       <c r="B207" s="36" t="s">
         <v>155</v>
       </c>

</xml_diff>